<commit_message>
[UPDATE] Budget File Merge
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Template.xlsx
+++ b/uploads/excel/RKAP Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4B0C4E-90E3-4A93-A0C8-FB453CD47AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B9A81D-224B-4334-B8C5-872F1A1E3F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="2700" windowWidth="16485" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1993,7 +1993,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="292" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2187,21 +2187,51 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="A5" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100.01</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100.02</v>
+      </c>
+      <c r="F5" s="4">
+        <v>100.03</v>
+      </c>
+      <c r="G5" s="4">
+        <v>100.04</v>
+      </c>
+      <c r="H5" s="4">
+        <v>100.05</v>
+      </c>
+      <c r="I5" s="4">
+        <v>100.06</v>
+      </c>
+      <c r="J5" s="4">
+        <v>100.07</v>
+      </c>
+      <c r="K5" s="4">
+        <v>100.08</v>
+      </c>
+      <c r="L5" s="4">
+        <v>100.09</v>
+      </c>
+      <c r="M5" s="4">
+        <v>100.1</v>
+      </c>
+      <c r="N5" s="4">
+        <v>100.11</v>
+      </c>
+      <c r="O5" s="4">
+        <v>100.12</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>

</xml_diff>